<commit_message>
Create activities Navegacao Faturas e Pesquisa Faturas
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://processor1-my.sharepoint.com/personal/tiago_martins_gotobiz_com_br/Documents/Documentos/uipath/Performer/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\OneDrive - Processor\Documentos\uipath\Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85C2FC7D-B0AB-4CE5-BB78-8FFC433E68EB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D59669-8DB7-44F3-BF95-D42132D1C3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-60" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>FilaFaturas</t>
+  </si>
+  <si>
+    <t>Demos</t>
+  </si>
+  <si>
+    <t>ACME_ProcurarFatura_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/invoices/search</t>
   </si>
 </sst>
 </file>
@@ -549,7 +558,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -609,7 +618,9 @@
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
@@ -645,7 +656,14 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>